<commit_message>
finish login log and attmepts limitation
</commit_message>
<xml_diff>
--- a/Release history.xlsx
+++ b/Release history.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Daily entry change: 8 input ---&gt; 2 input + table show daily timesheet</t>
   </si>
@@ -172,6 +172,18 @@
 对比原来的:
 ajax端 data: JSON.stringify(str) 
 python端: data = request.json 参考文件：Flask中Javascript和python数据互传.docx</t>
+  </si>
+  <si>
+    <t>准备linux环境</t>
+  </si>
+  <si>
+    <t>在vmware下安装ubuntu 18.04 desktop，user：ritchie/crm2020，administrator： root/crm2020，安装visualstudio，安装python：apt install python3.8，结果安装的是3.6.9；共享文件夹的时候在linux环境里需要使用mount语句</t>
+  </si>
+  <si>
+    <t>download运行错误是因为保存文件的文件夹不存在</t>
+  </si>
+  <si>
+    <t>login限制 登录大于3次错误限制1小时后登录，大于6次限制1天后登录。两个函数：authentication(user)用来检查是否是新用户，加锁、解锁；userrecrods(user, field)用来记录登录log，生成小时锁和24小时锁</t>
   </si>
 </sst>
 </file>
@@ -512,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +690,38 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44113</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44114</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add user expire date authentication
</commit_message>
<xml_diff>
--- a/Release history.xlsx
+++ b/Release history.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Daily entry change: 8 input ---&gt; 2 input + table show daily timesheet</t>
   </si>
@@ -174,23 +174,62 @@
 python端: data = request.json 参考文件：Flask中Javascript和python数据互传.docx</t>
   </si>
   <si>
-    <t>准备linux环境</t>
-  </si>
-  <si>
-    <t>在vmware下安装ubuntu 18.04 desktop，user：ritchie/crm2020，administrator： root/crm2020，安装visualstudio，安装python：apt install python3.8，结果安装的是3.6.9；共享文件夹的时候在linux环境里需要使用mount语句</t>
-  </si>
-  <si>
     <t>download运行错误是因为保存文件的文件夹不存在</t>
   </si>
   <si>
     <t>login限制 登录大于3次错误限制1小时后登录，大于6次限制1天后登录。两个函数：authentication(user)用来检查是否是新用户，加锁、解锁；userrecrods(user, field)用来记录登录log，生成小时锁和24小时锁</t>
+  </si>
+  <si>
+    <t>在vmware下安装ubuntu 18.04 desktop，user：ritchie/crm2020，administrator： root/crm2020，安装visualstudio，安装python：apt install python3.8，结果安装的是3.6.9；共享文件夹的时候在linux环境里需要使用mount语句. Sudo apt install virtualenv, reboot, sudo chmod 777 venv/bin/activate, source venv/bin/activate, pip install -r requirement.txt, FLASK_ENV="development", flask run --host=0.0.0.0. VMware共享host文件目录后，linux需要使用mount命令，/usr/bin/vmhgfs-fuse .host:/ /home/ritchie/Documents/shares -o subtype=vmhgfs-fuse,allow_other</t>
+  </si>
+  <si>
+    <t>准备linux环境, apt install net-tools, apt install python3.8, apt install python-pip, python3 --version, apt update</t>
+  </si>
+  <si>
+    <t>ubuntu error: when running "flask run " got error "ModuleNotFoundError: No module named 'thinter'" --- solution: 安装sudo apt-get install python3-tk即可，有的说要安装sudo apt-get install python3.6-tk，实际上不需要了</t>
+  </si>
+  <si>
+    <t>Tkinter是在python端的命令，所以窗口也就显示在服务器端，不会在client端browser上显示，改用flash在homepage上显示。注意flash只能显示render-templete或者redirect的网页上</t>
+  </si>
+  <si>
+    <t>linux环境下debug命令：export FLASK_APP=app, export FLASK_ENV=development</t>
+  </si>
+  <si>
+    <t>项目部署：见"文件CRM项目部署.docx"中"实际项目部署"和"How To Serve Flask Applications with Gunicorn and Nginx on Ubuntu 18.04"</t>
+  </si>
+  <si>
+    <t>user有效时间管理:1.user数据库表添加authorization栏 2.Register时候 authorization = int(time.time())+31536000)表示1年有效 3. Login时authentication身份验证添加au = db.session.query(User).filter(User.username == user).scalar()   if currenttime &gt; au.authorization:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Register/Profile/Edit Profile不显示的原因在于Register.html 中{% block </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>app_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>content %}, 去掉app_即可</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +250,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,10 +276,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -244,9 +292,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -524,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C35" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,20 +740,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44104</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="84" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44113</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,7 +761,7 @@
         <v>44114</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="36" x14ac:dyDescent="0.25">
@@ -719,11 +769,65 @@
         <v>44116</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44117</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44117</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="24" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44117</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="24" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44122</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish Send emails, encription utility.py
</commit_message>
<xml_diff>
--- a/Release history.xlsx
+++ b/Release history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ritchie\Documents\financial-computing-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Win10_Computer\financial-computing-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Daily entry change: 8 input ---&gt; 2 input + table show daily timesheet</t>
   </si>
@@ -224,12 +224,69 @@
       <t>content %}, 去掉app_即可</t>
     </r>
   </si>
+  <si>
+    <t>DELETE FROM tt WHERE timesheet_id in (
+SELECT timesheet_id FROM (SELECT ROW_NUMBER () OVER (ORDER BY timesheet_id) row, timesheet_id FROM tt) WHERE row &gt; 20
+);</t>
+  </si>
+  <si>
+    <t>新建financial-computing-app-deploy目录，删除#注释和文件</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">import uuid
+        print(hex(uuid.getnode())) &gt;&gt;&gt; 0x3085a9a93389
+        import socket    
+        hostname = socket.gethostname()    
+        IPAddr = socket.gethostbyname(hostname)    
+        print("Your Computer Name is:" + hostname)  &gt;&gt;&gt; Your Computer Name is:DESKTOP-GF5JV6T   
+        print("Your Computer IP Address is:" + IPAddr) &gt;&gt;&gt; Your Computer IP Address is:192.168.174.1
+        os.system('arp -a &gt; temp.txt')
+        import urllib.request
+        external_ip = urllib.request.urlopen('https://ident.me').read().decode('utf8')
+        print(external_ip) &gt;&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>142.114.13.75 外网IP</t>
+    </r>
+  </si>
+  <si>
+    <t>硬盘financial-computing-app中的sqlite表user已经加上了</t>
+  </si>
+  <si>
+    <t># Send emails （需要pip3 install Flask-Mail）
+app.config['DEBUG'] = True
+app.config['MAIL_SERVER'] ='smtp.gmail.com'
+app.config['MAIL_PORT'] = 465
+app.config['MAIL_USE_TLS'] = False
+app.config['MAIL_USE_SSL'] = True
+app.config['MAIL_USERNAME'] = 'brian.liu1618@gmail.com' # 如果验证失败，需要在google account里进行第三方登录允许设置
+app.config['MAIL_PASSWORD'] = 'chaplin525'
+app.config['MAIL_DEFAULT_SENDER'] = 'brian.liu1618@gmail.com'
+app.config['MAIL_MAX_EMAILS'] = None
+app.config['MAIL_ASCII_ATTACHMENTS'] = False
+#mail = Mail()
+#mail.init_app(app)
+# put following 4 lines in applications def
+# def send_email():
+#     mail = Mail(app) 放在应用里才行
+#     msg = Message('Hello', sender = 'brian.liu1618@gmail.com', recipients = ['brian.liu1618@gmail.com'])
+#     msg.body = "Hello Flask message sent from Flask-Mail"
+#     mail.send(msg)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +315,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -280,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -292,7 +367,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -574,17 +654,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C35" sqref="C34:C35"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="79.28515625" style="4" customWidth="1"/>
-    <col min="3" max="11" width="9.140625" style="1"/>
+    <col min="3" max="3" width="31" style="6" customWidth="1"/>
+    <col min="4" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,9 +903,38 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>44123</v>
-      </c>
-      <c r="B32" s="5"/>
+        <v>44124</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="48" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44127</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44127</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>